<commit_message>
Wip: integracion modificaicon formato
</commit_message>
<xml_diff>
--- a/imagenes_guardadas/archivo_con_firma.xlsx
+++ b/imagenes_guardadas/archivo_con_firma.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="58">
   <si>
     <t>Automóviles y Camiones Rivera, S.A. de C.V.</t>
   </si>
@@ -28,6 +28,9 @@
     <t>Fecha de realización:</t>
   </si>
   <si>
+    <t>22/01/2025</t>
+  </si>
+  <si>
     <t>No. de reporte:</t>
   </si>
   <si>
@@ -37,12 +40,12 @@
     <t>Programado</t>
   </si>
   <si>
+    <t>Solicitado</t>
+  </si>
+  <si>
     <t>✓</t>
   </si>
   <si>
-    <t>Solicitado</t>
-  </si>
-  <si>
     <t>Observación:</t>
   </si>
   <si>
@@ -52,7 +55,7 @@
     <t>Nombre del usuario:</t>
   </si>
   <si>
-    <t>Ángel Roberto Coronado</t>
+    <t>Ana Karen Sevilla Pulido</t>
   </si>
   <si>
     <t>Puesto:</t>
@@ -260,7 +263,7 @@
       <name val="CorpoS"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -270,6 +273,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC1F0C7"/>
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
@@ -324,15 +339,6 @@
     </border>
     <border>
       <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
@@ -398,6 +404,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
@@ -412,7 +427,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="69">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
     <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0"/>
     <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0"/>
@@ -427,25 +442,24 @@
     <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="1">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="1" numFmtId="14" fillId="2" borderId="5" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="0"/>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="5" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="4" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0"/>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="6" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0"/>
+    <xf xfId="0" fontId="5" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
+      <alignment vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
     <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="6" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="4" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0"/>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="7" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0"/>
-    <xf xfId="0" fontId="5" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
-      <alignment vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
     <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="7" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="8" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="9" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="10" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="1">
@@ -458,14 +472,14 @@
     <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="1">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="7" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
     <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="8" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="9" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="8" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0"/>
     <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="9" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0"/>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="10" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0"/>
     <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
@@ -475,20 +489,20 @@
     <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="4" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="11" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="10" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="6" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0"/>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="9" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="5" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0"/>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="8" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="5" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="5" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0"/>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="8" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0"/>
-    <xf xfId="0" fontId="1" numFmtId="4" fillId="2" borderId="9" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="0"/>
-    <xf xfId="0" fontId="1" numFmtId="4" fillId="2" borderId="10" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="11" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0"/>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="7" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0"/>
+    <xf xfId="0" fontId="1" numFmtId="4" fillId="2" borderId="8" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="0"/>
+    <xf xfId="0" fontId="1" numFmtId="4" fillId="2" borderId="9" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="1" numFmtId="4" fillId="2" borderId="0" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="0"/>
@@ -499,7 +513,54 @@
     <xf xfId="0" fontId="1" numFmtId="4" fillId="2" borderId="3" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="7" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="6" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="6" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="1">
+      <alignment vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="6" numFmtId="0" fillId="2" borderId="4" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="5" numFmtId="0" fillId="3" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="1">
+      <alignment vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="5" numFmtId="0" fillId="3" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="14" fillId="4" borderId="11" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="0"/>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="4" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0"/>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="6" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="11" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="5" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="4" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="4" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="6" numFmtId="0" fillId="4" borderId="12" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="6" numFmtId="0" fillId="4" borderId="11" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="6" numFmtId="0" fillId="2" borderId="4" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="6" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="4" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -508,56 +569,29 @@
     <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="1">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="5" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="3" borderId="11" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="6" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="6" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="3" borderId="5" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="4" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="49" fillId="2" borderId="5" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="4" borderId="11" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="1" numFmtId="49" fillId="2" borderId="6" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="4" borderId="5" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="4" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="1" numFmtId="49" fillId="3" borderId="11" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="1">
+    <xf xfId="0" fontId="1" numFmtId="49" fillId="3" borderId="5" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="7" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="7" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="7" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="6" numFmtId="0" fillId="2" borderId="5" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="6" numFmtId="0" fillId="2" borderId="12" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="6" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="1">
-      <alignment vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="6" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="6" numFmtId="0" fillId="2" borderId="4" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="6" numFmtId="0" fillId="2" borderId="4" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -610,9 +644,9 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
+      <xdr:colOff>571500</xdr:colOff>
       <xdr:row>73</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1019175" cy="514350"/>
     <xdr:pic>
@@ -966,15 +1000,15 @@
   </sheetPr>
   <dimension ref="A1:N79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" view="pageBreakPreview" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="Q77" sqref="Q77"/>
+    <sheetView tabSelected="1" workbookViewId="0" view="pageBreakPreview" showGridLines="true" showRowColHeaders="1" topLeftCell="A65">
+      <selection activeCell="B76" sqref="B76:C76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="1.42578125" customWidth="true" style="1"/>
     <col min="2" max="2" width="11.42578125" customWidth="true" style="1"/>
-    <col min="3" max="3" width="11.42578125" customWidth="true" style="1"/>
+    <col min="3" max="3" width="20.85546875" customWidth="true" style="1"/>
     <col min="4" max="4" width="1.28515625" customWidth="true" style="1"/>
     <col min="5" max="5" width="1.42578125" customWidth="true" style="1"/>
     <col min="6" max="6" width="11.42578125" customWidth="true" style="1"/>
@@ -1019,48 +1053,49 @@
       <c r="M6" s="7"/>
     </row>
     <row r="7" spans="1:14">
-      <c r="B7" s="47" t="s">
+      <c r="B7" s="52" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="48"/>
-      <c r="D7" s="48"/>
-      <c r="E7" s="48"/>
-      <c r="F7" s="10">
-        <v>45672</v>
-      </c>
-      <c r="H7" s="48" t="s">
+      <c r="C7" s="53"/>
+      <c r="D7" s="53"/>
+      <c r="E7" s="53"/>
+      <c r="F7" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="I7" s="48"/>
-      <c r="J7" s="48"/>
-      <c r="K7" s="48"/>
-      <c r="L7" s="45" t="s">
+      <c r="H7" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="M7" s="46"/>
+      <c r="I7" s="53"/>
+      <c r="J7" s="53"/>
+      <c r="K7" s="53"/>
+      <c r="L7" s="61" t="s">
+        <v>5</v>
+      </c>
+      <c r="M7" s="64"/>
     </row>
     <row r="8" spans="1:14" customHeight="1" ht="7.5">
-      <c r="B8" s="12"/>
-      <c r="M8" s="13"/>
+      <c r="B8" s="11"/>
+      <c r="M8" s="12"/>
     </row>
     <row r="9" spans="1:14" customHeight="1" ht="13.5">
       <c r="A9" s="9"/>
-      <c r="B9" s="47" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="48"/>
-      <c r="D9" s="1" t="s">
+      <c r="B9" s="52" t="s">
         <v>6</v>
       </c>
+      <c r="C9" s="53"/>
+      <c r="D9" s="47"/>
       <c r="F9" s="9"/>
       <c r="G9" s="9"/>
-      <c r="H9" s="48" t="s">
+      <c r="H9" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="I9" s="48"/>
-      <c r="K9" s="14"/>
+      <c r="I9" s="53"/>
+      <c r="J9" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="K9" s="13"/>
       <c r="L9" s="9"/>
-      <c r="M9" s="15"/>
+      <c r="M9" s="14"/>
     </row>
     <row r="10" spans="1:14" customHeight="1" ht="7.5">
       <c r="A10" s="9"/>
@@ -1075,41 +1110,41 @@
       <c r="J10" s="9"/>
       <c r="K10" s="9"/>
       <c r="L10" s="9"/>
-      <c r="M10" s="15"/>
+      <c r="M10" s="14"/>
     </row>
     <row r="11" spans="1:14">
       <c r="A11" s="9"/>
-      <c r="B11" s="47" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="48"/>
+      <c r="B11" s="52" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="53"/>
       <c r="D11" s="9"/>
-      <c r="E11" s="45" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11" s="45"/>
-      <c r="G11" s="45"/>
-      <c r="H11" s="45"/>
-      <c r="I11" s="45"/>
-      <c r="J11" s="45"/>
-      <c r="K11" s="45"/>
-      <c r="L11" s="45"/>
-      <c r="M11" s="46"/>
+      <c r="E11" s="65" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="65"/>
+      <c r="G11" s="65"/>
+      <c r="H11" s="65"/>
+      <c r="I11" s="65"/>
+      <c r="J11" s="65"/>
+      <c r="K11" s="65"/>
+      <c r="L11" s="65"/>
+      <c r="M11" s="66"/>
     </row>
     <row r="12" spans="1:14" customHeight="1" ht="7.5">
       <c r="A12" s="9"/>
-      <c r="B12" s="16"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="17"/>
-      <c r="I12" s="17"/>
-      <c r="J12" s="17"/>
-      <c r="K12" s="17"/>
-      <c r="L12" s="17"/>
-      <c r="M12" s="18"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="16"/>
+      <c r="J12" s="16"/>
+      <c r="K12" s="16"/>
+      <c r="L12" s="16"/>
+      <c r="M12" s="17"/>
     </row>
     <row r="13" spans="1:14" customHeight="1" ht="7.5">
       <c r="A13" s="9"/>
@@ -1124,10 +1159,10 @@
       <c r="J13" s="9"/>
       <c r="K13" s="9"/>
       <c r="L13" s="9"/>
-      <c r="M13" s="19"/>
+      <c r="M13" s="18"/>
     </row>
     <row r="14" spans="1:14" customHeight="1" ht="7.5">
-      <c r="B14" s="20"/>
+      <c r="B14" s="19"/>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
@@ -1142,133 +1177,133 @@
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="9"/>
-      <c r="B15" s="43" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" s="44"/>
-      <c r="D15" s="22"/>
+      <c r="B15" s="59" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="60"/>
+      <c r="D15" s="21"/>
       <c r="E15" s="9"/>
-      <c r="F15" s="45" t="s">
-        <v>11</v>
-      </c>
-      <c r="G15" s="45"/>
-      <c r="H15" s="45"/>
-      <c r="I15" s="45"/>
-      <c r="J15" s="45"/>
-      <c r="K15" s="45"/>
-      <c r="L15" s="45"/>
-      <c r="M15" s="46"/>
+      <c r="F15" s="65" t="s">
+        <v>12</v>
+      </c>
+      <c r="G15" s="65"/>
+      <c r="H15" s="65"/>
+      <c r="I15" s="65"/>
+      <c r="J15" s="65"/>
+      <c r="K15" s="65"/>
+      <c r="L15" s="65"/>
+      <c r="M15" s="66"/>
     </row>
     <row r="16" spans="1:14" customHeight="1" ht="7.5">
-      <c r="B16" s="12"/>
-      <c r="M16" s="13"/>
+      <c r="B16" s="11"/>
+      <c r="M16" s="12"/>
     </row>
     <row r="17" spans="1:14">
-      <c r="B17" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="C17" s="45" t="s">
+      <c r="B17" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="D17" s="45"/>
-      <c r="E17" s="45"/>
-      <c r="F17" s="45"/>
-      <c r="H17" s="44" t="s">
+      <c r="C17" s="61" t="s">
         <v>14</v>
       </c>
-      <c r="I17" s="44"/>
-      <c r="J17" s="49" t="s">
+      <c r="D17" s="61"/>
+      <c r="E17" s="61"/>
+      <c r="F17" s="61"/>
+      <c r="H17" s="60" t="s">
         <v>15</v>
       </c>
-      <c r="K17" s="49"/>
-      <c r="L17" s="49"/>
-      <c r="M17" s="50"/>
+      <c r="I17" s="60"/>
+      <c r="J17" s="67" t="s">
+        <v>16</v>
+      </c>
+      <c r="K17" s="67"/>
+      <c r="L17" s="67"/>
+      <c r="M17" s="68"/>
     </row>
     <row r="18" spans="1:14" customHeight="1" ht="7.5">
-      <c r="B18" s="12"/>
-      <c r="M18" s="13"/>
+      <c r="B18" s="11"/>
+      <c r="M18" s="12"/>
     </row>
     <row r="19" spans="1:14">
       <c r="A19" s="9"/>
-      <c r="B19" s="43" t="s">
-        <v>16</v>
-      </c>
-      <c r="C19" s="44"/>
-      <c r="D19" s="45" t="s">
+      <c r="B19" s="59" t="s">
         <v>17</v>
       </c>
-      <c r="E19" s="45"/>
-      <c r="F19" s="45"/>
-      <c r="H19" s="44" t="s">
+      <c r="C19" s="60"/>
+      <c r="D19" s="61" t="s">
         <v>18</v>
       </c>
-      <c r="I19" s="44"/>
-      <c r="J19" s="45"/>
-      <c r="K19" s="45"/>
-      <c r="L19" s="45"/>
-      <c r="M19" s="46"/>
+      <c r="E19" s="61"/>
+      <c r="F19" s="61"/>
+      <c r="H19" s="60" t="s">
+        <v>19</v>
+      </c>
+      <c r="I19" s="60"/>
+      <c r="J19" s="50"/>
+      <c r="K19" s="50"/>
+      <c r="L19" s="50"/>
+      <c r="M19" s="51"/>
     </row>
     <row r="20" spans="1:14" customHeight="1" ht="7.5">
-      <c r="B20" s="12"/>
-      <c r="M20" s="13"/>
+      <c r="B20" s="11"/>
+      <c r="M20" s="12"/>
     </row>
     <row r="21" spans="1:14">
       <c r="A21" s="9"/>
-      <c r="B21" s="43" t="s">
-        <v>19</v>
-      </c>
-      <c r="C21" s="44"/>
-      <c r="D21" s="45" t="s">
+      <c r="B21" s="59" t="s">
         <v>20</v>
       </c>
-      <c r="E21" s="45"/>
-      <c r="F21" s="45"/>
-      <c r="H21" s="22" t="s">
+      <c r="C21" s="60"/>
+      <c r="D21" s="61" t="s">
         <v>21</v>
       </c>
-      <c r="I21" s="22"/>
-      <c r="J21" s="45"/>
-      <c r="K21" s="45"/>
-      <c r="L21" s="45"/>
-      <c r="M21" s="46"/>
+      <c r="E21" s="61"/>
+      <c r="F21" s="61"/>
+      <c r="H21" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="I21" s="21"/>
+      <c r="J21" s="50"/>
+      <c r="K21" s="50"/>
+      <c r="L21" s="50"/>
+      <c r="M21" s="51"/>
     </row>
     <row r="22" spans="1:14" customHeight="1" ht="7.5">
-      <c r="B22" s="12"/>
-      <c r="M22" s="13"/>
+      <c r="B22" s="11"/>
+      <c r="M22" s="12"/>
     </row>
     <row r="23" spans="1:14">
       <c r="A23" s="9"/>
-      <c r="B23" s="47" t="s">
-        <v>8</v>
-      </c>
-      <c r="C23" s="48"/>
+      <c r="B23" s="52" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" s="53"/>
       <c r="D23" s="9"/>
-      <c r="E23" s="45" t="s">
-        <v>22</v>
-      </c>
-      <c r="F23" s="45"/>
-      <c r="G23" s="45"/>
-      <c r="H23" s="45"/>
-      <c r="I23" s="45"/>
-      <c r="J23" s="45"/>
-      <c r="K23" s="45"/>
-      <c r="L23" s="45"/>
-      <c r="M23" s="46"/>
+      <c r="E23" s="50" t="s">
+        <v>23</v>
+      </c>
+      <c r="F23" s="50"/>
+      <c r="G23" s="50"/>
+      <c r="H23" s="50"/>
+      <c r="I23" s="50"/>
+      <c r="J23" s="50"/>
+      <c r="K23" s="50"/>
+      <c r="L23" s="50"/>
+      <c r="M23" s="51"/>
     </row>
     <row r="24" spans="1:14" customHeight="1" ht="7.5">
       <c r="A24" s="9"/>
-      <c r="B24" s="23"/>
-      <c r="C24" s="24"/>
-      <c r="D24" s="24"/>
-      <c r="E24" s="17"/>
-      <c r="F24" s="25"/>
-      <c r="G24" s="25"/>
-      <c r="H24" s="25"/>
-      <c r="I24" s="25"/>
-      <c r="J24" s="25"/>
-      <c r="K24" s="25"/>
-      <c r="L24" s="25"/>
-      <c r="M24" s="26"/>
+      <c r="B24" s="22"/>
+      <c r="C24" s="23"/>
+      <c r="D24" s="23"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="24"/>
+      <c r="G24" s="24"/>
+      <c r="H24" s="24"/>
+      <c r="I24" s="24"/>
+      <c r="J24" s="24"/>
+      <c r="K24" s="24"/>
+      <c r="L24" s="24"/>
+      <c r="M24" s="25"/>
     </row>
     <row r="25" spans="1:14" customHeight="1" ht="7.5">
       <c r="A25" s="9"/>
@@ -1279,10 +1314,10 @@
     </row>
     <row r="26" spans="1:14" customHeight="1" ht="7.5">
       <c r="A26" s="9"/>
-      <c r="B26" s="27"/>
-      <c r="C26" s="28"/>
-      <c r="D26" s="28"/>
-      <c r="E26" s="28"/>
+      <c r="B26" s="26"/>
+      <c r="C26" s="27"/>
+      <c r="D26" s="27"/>
+      <c r="E26" s="27"/>
       <c r="F26" s="6"/>
       <c r="G26" s="6"/>
       <c r="H26" s="6"/>
@@ -1293,21 +1328,21 @@
       <c r="M26" s="7"/>
     </row>
     <row r="27" spans="1:14">
-      <c r="B27" s="51" t="s">
-        <v>23</v>
-      </c>
-      <c r="C27" s="52"/>
-      <c r="D27" s="52"/>
-      <c r="E27" s="52"/>
-      <c r="F27" s="52"/>
-      <c r="H27" s="52" t="s">
+      <c r="B27" s="54" t="s">
         <v>24</v>
       </c>
-      <c r="I27" s="52"/>
-      <c r="J27" s="52"/>
-      <c r="K27" s="52"/>
-      <c r="L27" s="52"/>
-      <c r="M27" s="53"/>
+      <c r="C27" s="48"/>
+      <c r="D27" s="48"/>
+      <c r="E27" s="48"/>
+      <c r="F27" s="48"/>
+      <c r="H27" s="48" t="s">
+        <v>25</v>
+      </c>
+      <c r="I27" s="48"/>
+      <c r="J27" s="48"/>
+      <c r="K27" s="48"/>
+      <c r="L27" s="48"/>
+      <c r="M27" s="49"/>
     </row>
     <row r="28" spans="1:14" customHeight="1" ht="7.5">
       <c r="A28" s="9"/>
@@ -1315,33 +1350,31 @@
       <c r="C28" s="9"/>
       <c r="D28" s="9"/>
       <c r="E28" s="9"/>
-      <c r="M28" s="13"/>
+      <c r="M28" s="12"/>
     </row>
     <row r="29" spans="1:14" customHeight="1" ht="13.5">
       <c r="A29" s="9"/>
-      <c r="B29" s="47" t="s">
-        <v>25</v>
-      </c>
-      <c r="C29" s="48"/>
+      <c r="B29" s="52" t="s">
+        <v>26</v>
+      </c>
+      <c r="C29" s="53"/>
       <c r="D29" s="9"/>
-      <c r="E29" s="14" t="s">
-        <v>6</v>
-      </c>
+      <c r="E29" s="44"/>
       <c r="F29" s="9"/>
-      <c r="G29" s="48" t="s">
-        <v>26</v>
-      </c>
-      <c r="H29" s="48"/>
-      <c r="I29" s="48"/>
+      <c r="G29" s="53" t="s">
+        <v>27</v>
+      </c>
+      <c r="H29" s="53"/>
+      <c r="I29" s="53"/>
       <c r="J29" s="9"/>
-      <c r="K29" s="14"/>
-      <c r="L29" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="M29" s="54"/>
+      <c r="K29" s="13"/>
+      <c r="L29" s="44" t="s">
+        <v>8</v>
+      </c>
+      <c r="M29" s="62"/>
     </row>
     <row r="30" spans="1:14" customHeight="1" ht="7.5">
-      <c r="B30" s="29"/>
+      <c r="B30" s="28"/>
       <c r="F30" s="9"/>
       <c r="G30" s="9"/>
       <c r="H30" s="9"/>
@@ -1349,30 +1382,28 @@
       <c r="J30" s="9"/>
       <c r="K30" s="9"/>
       <c r="L30" s="9"/>
-      <c r="M30" s="55"/>
+      <c r="M30" s="63"/>
     </row>
     <row r="31" spans="1:14" customHeight="1" ht="13.5">
       <c r="A31" s="9"/>
-      <c r="B31" s="47" t="s">
-        <v>27</v>
-      </c>
-      <c r="C31" s="48"/>
+      <c r="B31" s="52" t="s">
+        <v>28</v>
+      </c>
+      <c r="C31" s="53"/>
       <c r="D31" s="9"/>
-      <c r="E31" s="14" t="s">
-        <v>6</v>
-      </c>
+      <c r="E31" s="44"/>
       <c r="F31" s="9"/>
-      <c r="G31" s="48" t="s">
-        <v>28</v>
-      </c>
-      <c r="H31" s="48"/>
-      <c r="I31" s="48"/>
+      <c r="G31" s="53" t="s">
+        <v>29</v>
+      </c>
+      <c r="H31" s="53"/>
+      <c r="I31" s="53"/>
       <c r="J31" s="9"/>
-      <c r="K31" s="14"/>
-      <c r="L31" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="M31" s="55"/>
+      <c r="K31" s="13"/>
+      <c r="L31" s="44" t="s">
+        <v>8</v>
+      </c>
+      <c r="M31" s="63"/>
     </row>
     <row r="32" spans="1:14" customHeight="1" ht="7.5">
       <c r="B32" s="8"/>
@@ -1383,31 +1414,31 @@
       <c r="J32" s="9"/>
       <c r="K32" s="9"/>
       <c r="L32" s="9"/>
-      <c r="M32" s="13"/>
+      <c r="M32" s="12"/>
     </row>
     <row r="33" spans="1:14" customHeight="1" ht="13.5">
       <c r="A33" s="9"/>
-      <c r="B33" s="47" t="s">
-        <v>29</v>
-      </c>
-      <c r="C33" s="48"/>
+      <c r="B33" s="52" t="s">
+        <v>30</v>
+      </c>
+      <c r="C33" s="53"/>
       <c r="D33" s="9"/>
-      <c r="E33" s="14" t="s">
-        <v>6</v>
+      <c r="E33" s="44" t="s">
+        <v>8</v>
       </c>
       <c r="F33" s="9"/>
-      <c r="G33" s="48" t="s">
-        <v>30</v>
-      </c>
-      <c r="H33" s="48"/>
-      <c r="I33" s="48"/>
+      <c r="G33" s="53" t="s">
+        <v>31</v>
+      </c>
+      <c r="H33" s="53"/>
+      <c r="I33" s="53"/>
       <c r="J33" s="9"/>
-      <c r="K33" s="30"/>
+      <c r="K33" s="29"/>
       <c r="L33" s="9"/>
-      <c r="M33" s="31"/>
+      <c r="M33" s="30"/>
     </row>
     <row r="34" spans="1:14" customHeight="1" ht="7.5">
-      <c r="B34" s="29"/>
+      <c r="B34" s="28"/>
       <c r="F34" s="9"/>
       <c r="G34" s="9"/>
       <c r="H34" s="9"/>
@@ -1415,88 +1446,88 @@
       <c r="J34" s="9"/>
       <c r="K34" s="9"/>
       <c r="L34" s="9"/>
-      <c r="M34" s="15"/>
+      <c r="M34" s="14"/>
     </row>
     <row r="35" spans="1:14" customHeight="1" ht="13.5">
       <c r="A35" s="9"/>
-      <c r="B35" s="47" t="s">
-        <v>31</v>
-      </c>
-      <c r="C35" s="48"/>
+      <c r="B35" s="52" t="s">
+        <v>32</v>
+      </c>
+      <c r="C35" s="53"/>
       <c r="D35" s="9"/>
-      <c r="E35" s="14"/>
-      <c r="G35" s="48" t="s">
-        <v>32</v>
-      </c>
-      <c r="H35" s="48"/>
-      <c r="I35" s="48"/>
+      <c r="E35" s="13"/>
+      <c r="G35" s="53" t="s">
+        <v>33</v>
+      </c>
+      <c r="H35" s="53"/>
+      <c r="I35" s="53"/>
       <c r="J35" s="9"/>
-      <c r="K35" s="30"/>
+      <c r="K35" s="29"/>
       <c r="L35" s="9"/>
-      <c r="M35" s="11"/>
+      <c r="M35" s="10"/>
     </row>
     <row r="36" spans="1:14" customHeight="1" ht="7.5">
-      <c r="B36" s="29"/>
-      <c r="F36" s="19"/>
-      <c r="G36" s="19"/>
-      <c r="H36" s="19"/>
-      <c r="I36" s="19"/>
-      <c r="J36" s="19"/>
-      <c r="K36" s="19"/>
-      <c r="L36" s="19"/>
-      <c r="M36" s="15"/>
+      <c r="B36" s="28"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="18"/>
+      <c r="H36" s="18"/>
+      <c r="I36" s="18"/>
+      <c r="J36" s="18"/>
+      <c r="K36" s="18"/>
+      <c r="L36" s="18"/>
+      <c r="M36" s="14"/>
     </row>
     <row r="37" spans="1:14" customHeight="1" ht="13.5">
       <c r="A37" s="9"/>
-      <c r="B37" s="47" t="s">
-        <v>33</v>
-      </c>
-      <c r="C37" s="48"/>
+      <c r="B37" s="52" t="s">
+        <v>34</v>
+      </c>
+      <c r="C37" s="53"/>
       <c r="D37" s="9"/>
-      <c r="E37" s="14"/>
-      <c r="F37" s="19"/>
-      <c r="G37" s="48" t="s">
-        <v>34</v>
-      </c>
-      <c r="H37" s="48"/>
-      <c r="I37" s="48"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="18"/>
+      <c r="G37" s="53" t="s">
+        <v>35</v>
+      </c>
+      <c r="H37" s="53"/>
+      <c r="I37" s="53"/>
       <c r="J37" s="9"/>
-      <c r="K37" s="30"/>
-      <c r="L37" s="19"/>
-      <c r="M37" s="11"/>
+      <c r="K37" s="29"/>
+      <c r="L37" s="18"/>
+      <c r="M37" s="10"/>
     </row>
     <row r="38" spans="1:14" customHeight="1" ht="7.5">
       <c r="A38" s="9"/>
-      <c r="B38" s="16"/>
-      <c r="C38" s="17"/>
-      <c r="D38" s="17"/>
-      <c r="E38" s="17"/>
-      <c r="F38" s="32"/>
-      <c r="G38" s="32"/>
-      <c r="H38" s="32"/>
-      <c r="I38" s="32"/>
-      <c r="J38" s="32"/>
-      <c r="K38" s="32"/>
-      <c r="L38" s="32"/>
-      <c r="M38" s="18"/>
+      <c r="B38" s="15"/>
+      <c r="C38" s="16"/>
+      <c r="D38" s="16"/>
+      <c r="E38" s="16"/>
+      <c r="F38" s="31"/>
+      <c r="G38" s="31"/>
+      <c r="H38" s="31"/>
+      <c r="I38" s="31"/>
+      <c r="J38" s="31"/>
+      <c r="K38" s="31"/>
+      <c r="L38" s="31"/>
+      <c r="M38" s="17"/>
     </row>
     <row r="39" spans="1:14" customHeight="1" ht="7.5">
-      <c r="A39" s="19"/>
-      <c r="B39" s="19"/>
-      <c r="C39" s="19"/>
-      <c r="D39" s="19"/>
-      <c r="E39" s="19"/>
-      <c r="F39" s="19"/>
-      <c r="G39" s="19"/>
-      <c r="H39" s="19"/>
-      <c r="I39" s="19"/>
-      <c r="J39" s="19"/>
-      <c r="K39" s="19"/>
-      <c r="L39" s="19"/>
-      <c r="M39" s="19"/>
+      <c r="A39" s="18"/>
+      <c r="B39" s="18"/>
+      <c r="C39" s="18"/>
+      <c r="D39" s="18"/>
+      <c r="E39" s="18"/>
+      <c r="F39" s="18"/>
+      <c r="G39" s="18"/>
+      <c r="H39" s="18"/>
+      <c r="I39" s="18"/>
+      <c r="J39" s="18"/>
+      <c r="K39" s="18"/>
+      <c r="L39" s="18"/>
+      <c r="M39" s="18"/>
     </row>
     <row r="40" spans="1:14" customHeight="1" ht="7.5">
-      <c r="B40" s="20"/>
+      <c r="B40" s="19"/>
       <c r="C40" s="6"/>
       <c r="D40" s="6"/>
       <c r="E40" s="6"/>
@@ -1510,301 +1541,301 @@
       <c r="M40" s="7"/>
     </row>
     <row r="41" spans="1:14">
-      <c r="B41" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="M41" s="13"/>
+      <c r="B41" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="M41" s="12"/>
     </row>
     <row r="42" spans="1:14">
-      <c r="B42" s="12"/>
-      <c r="F42" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="H42" s="19" t="s">
+      <c r="B42" s="11"/>
+      <c r="F42" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="M42" s="15"/>
+      <c r="H42" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="M42" s="14"/>
     </row>
     <row r="43" spans="1:14" customHeight="1" ht="13.5">
-      <c r="B43" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="F43" s="33" t="s">
-        <v>6</v>
-      </c>
-      <c r="H43" s="34"/>
-      <c r="I43" s="34"/>
-      <c r="J43" s="34"/>
-      <c r="K43" s="34"/>
-      <c r="L43" s="34"/>
-      <c r="M43" s="11"/>
+      <c r="B43" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="F43" s="45" t="s">
+        <v>8</v>
+      </c>
+      <c r="H43" s="33"/>
+      <c r="I43" s="33"/>
+      <c r="J43" s="33"/>
+      <c r="K43" s="33"/>
+      <c r="L43" s="33"/>
+      <c r="M43" s="10"/>
     </row>
     <row r="44" spans="1:14" customHeight="1" ht="3.75">
-      <c r="B44" s="12"/>
-      <c r="M44" s="13"/>
+      <c r="B44" s="11"/>
+      <c r="M44" s="12"/>
     </row>
     <row r="45" spans="1:14" customHeight="1" ht="13.5">
-      <c r="B45" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="F45" s="33" t="s">
-        <v>6</v>
-      </c>
-      <c r="H45" s="34"/>
-      <c r="I45" s="34"/>
-      <c r="J45" s="34"/>
-      <c r="K45" s="34"/>
-      <c r="L45" s="34"/>
-      <c r="M45" s="11"/>
+      <c r="B45" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="F45" s="45" t="s">
+        <v>8</v>
+      </c>
+      <c r="H45" s="33"/>
+      <c r="I45" s="33"/>
+      <c r="J45" s="33"/>
+      <c r="K45" s="33"/>
+      <c r="L45" s="33"/>
+      <c r="M45" s="10"/>
     </row>
     <row r="46" spans="1:14" customHeight="1" ht="3.75">
-      <c r="B46" s="12"/>
-      <c r="M46" s="13"/>
+      <c r="B46" s="11"/>
+      <c r="M46" s="12"/>
     </row>
     <row r="47" spans="1:14" customHeight="1" ht="13.5">
-      <c r="B47" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="F47" s="33" t="s">
-        <v>6</v>
-      </c>
-      <c r="H47" s="34"/>
-      <c r="I47" s="34"/>
-      <c r="J47" s="34"/>
-      <c r="K47" s="34"/>
-      <c r="L47" s="34"/>
-      <c r="M47" s="11"/>
+      <c r="B47" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="F47" s="45" t="s">
+        <v>8</v>
+      </c>
+      <c r="H47" s="33"/>
+      <c r="I47" s="33"/>
+      <c r="J47" s="33"/>
+      <c r="K47" s="33"/>
+      <c r="L47" s="33"/>
+      <c r="M47" s="10"/>
     </row>
     <row r="48" spans="1:14" customHeight="1" ht="3.75">
-      <c r="B48" s="12"/>
-      <c r="M48" s="13"/>
+      <c r="B48" s="11"/>
+      <c r="M48" s="12"/>
     </row>
     <row r="49" spans="1:14" customHeight="1" ht="13.5">
-      <c r="B49" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="F49" s="33" t="s">
-        <v>6</v>
-      </c>
-      <c r="H49" s="34"/>
-      <c r="I49" s="34"/>
-      <c r="J49" s="34"/>
-      <c r="K49" s="34"/>
-      <c r="L49" s="34"/>
-      <c r="M49" s="11"/>
+      <c r="B49" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="F49" s="45" t="s">
+        <v>8</v>
+      </c>
+      <c r="H49" s="33"/>
+      <c r="I49" s="33"/>
+      <c r="J49" s="33"/>
+      <c r="K49" s="33"/>
+      <c r="L49" s="33"/>
+      <c r="M49" s="10"/>
     </row>
     <row r="50" spans="1:14" customHeight="1" ht="3.75">
-      <c r="B50" s="12"/>
-      <c r="M50" s="13"/>
+      <c r="B50" s="11"/>
+      <c r="M50" s="12"/>
     </row>
     <row r="51" spans="1:14" customHeight="1" ht="13.5">
-      <c r="B51" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="F51" s="33" t="s">
-        <v>6</v>
-      </c>
-      <c r="H51" s="34"/>
-      <c r="I51" s="34"/>
-      <c r="J51" s="34"/>
-      <c r="K51" s="34"/>
-      <c r="L51" s="34"/>
-      <c r="M51" s="11"/>
+      <c r="B51" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="F51" s="45" t="s">
+        <v>8</v>
+      </c>
+      <c r="H51" s="33"/>
+      <c r="I51" s="33"/>
+      <c r="J51" s="33"/>
+      <c r="K51" s="33"/>
+      <c r="L51" s="33"/>
+      <c r="M51" s="10"/>
     </row>
     <row r="52" spans="1:14" customHeight="1" ht="7.5">
-      <c r="B52" s="35"/>
-      <c r="C52" s="25"/>
-      <c r="D52" s="25"/>
-      <c r="E52" s="25"/>
-      <c r="F52" s="36"/>
-      <c r="G52" s="36"/>
-      <c r="H52" s="36"/>
-      <c r="I52" s="36"/>
-      <c r="J52" s="36"/>
-      <c r="K52" s="36"/>
-      <c r="L52" s="36"/>
-      <c r="M52" s="37"/>
+      <c r="B52" s="34"/>
+      <c r="C52" s="24"/>
+      <c r="D52" s="24"/>
+      <c r="E52" s="24"/>
+      <c r="F52" s="35"/>
+      <c r="G52" s="35"/>
+      <c r="H52" s="35"/>
+      <c r="I52" s="35"/>
+      <c r="J52" s="35"/>
+      <c r="K52" s="35"/>
+      <c r="L52" s="35"/>
+      <c r="M52" s="36"/>
     </row>
     <row r="53" spans="1:14" customHeight="1" ht="7.5">
-      <c r="F53" s="38"/>
-      <c r="G53" s="38"/>
-      <c r="H53" s="38"/>
-      <c r="I53" s="38"/>
-      <c r="J53" s="38"/>
-      <c r="K53" s="38"/>
-      <c r="L53" s="38"/>
-      <c r="M53" s="39"/>
+      <c r="F53" s="37"/>
+      <c r="G53" s="37"/>
+      <c r="H53" s="37"/>
+      <c r="I53" s="37"/>
+      <c r="J53" s="37"/>
+      <c r="K53" s="37"/>
+      <c r="L53" s="37"/>
+      <c r="M53" s="38"/>
     </row>
     <row r="54" spans="1:14" customHeight="1" ht="7.5">
-      <c r="B54" s="20"/>
+      <c r="B54" s="19"/>
       <c r="C54" s="6"/>
       <c r="D54" s="6"/>
       <c r="E54" s="6"/>
-      <c r="F54" s="40"/>
-      <c r="G54" s="40"/>
-      <c r="H54" s="40"/>
-      <c r="I54" s="40"/>
-      <c r="J54" s="40"/>
-      <c r="K54" s="40"/>
-      <c r="L54" s="40"/>
-      <c r="M54" s="41"/>
+      <c r="F54" s="39"/>
+      <c r="G54" s="39"/>
+      <c r="H54" s="39"/>
+      <c r="I54" s="39"/>
+      <c r="J54" s="39"/>
+      <c r="K54" s="39"/>
+      <c r="L54" s="39"/>
+      <c r="M54" s="40"/>
     </row>
     <row r="55" spans="1:14">
-      <c r="B55" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="F55" s="19"/>
-      <c r="H55" s="19"/>
-      <c r="M55" s="15"/>
+      <c r="B55" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="F55" s="18"/>
+      <c r="H55" s="18"/>
+      <c r="M55" s="14"/>
     </row>
     <row r="56" spans="1:14" customHeight="1" ht="12">
-      <c r="B56" s="12"/>
-      <c r="F56" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="H56" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="M56" s="15"/>
+      <c r="B56" s="11"/>
+      <c r="F56" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="H56" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="M56" s="14"/>
     </row>
     <row r="57" spans="1:14" customHeight="1" ht="13.5">
-      <c r="B57" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="F57" s="33" t="s">
-        <v>6</v>
-      </c>
-      <c r="H57" s="34"/>
-      <c r="I57" s="34"/>
-      <c r="J57" s="34"/>
-      <c r="K57" s="34"/>
-      <c r="L57" s="34"/>
-      <c r="M57" s="11"/>
+      <c r="B57" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="F57" s="45" t="s">
+        <v>8</v>
+      </c>
+      <c r="H57" s="33"/>
+      <c r="I57" s="33"/>
+      <c r="J57" s="33"/>
+      <c r="K57" s="33"/>
+      <c r="L57" s="33"/>
+      <c r="M57" s="10"/>
     </row>
     <row r="58" spans="1:14" customHeight="1" ht="3.75">
-      <c r="B58" s="12"/>
-      <c r="F58" s="19"/>
-      <c r="M58" s="13"/>
+      <c r="B58" s="11"/>
+      <c r="F58" s="18"/>
+      <c r="M58" s="12"/>
     </row>
     <row r="59" spans="1:14" customHeight="1" ht="13.5">
-      <c r="B59" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="F59" s="33" t="s">
-        <v>6</v>
-      </c>
-      <c r="H59" s="34"/>
-      <c r="I59" s="34"/>
-      <c r="J59" s="34"/>
-      <c r="K59" s="34"/>
-      <c r="L59" s="34"/>
-      <c r="M59" s="11"/>
+      <c r="B59" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="F59" s="45" t="s">
+        <v>8</v>
+      </c>
+      <c r="H59" s="33"/>
+      <c r="I59" s="33"/>
+      <c r="J59" s="33"/>
+      <c r="K59" s="33"/>
+      <c r="L59" s="33"/>
+      <c r="M59" s="10"/>
     </row>
     <row r="60" spans="1:14" customHeight="1" ht="3.75">
-      <c r="B60" s="12"/>
-      <c r="F60" s="19"/>
-      <c r="M60" s="13"/>
+      <c r="B60" s="11"/>
+      <c r="F60" s="18"/>
+      <c r="M60" s="12"/>
     </row>
     <row r="61" spans="1:14" customHeight="1" ht="13.5">
-      <c r="B61" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="F61" s="33"/>
-      <c r="H61" s="34"/>
-      <c r="I61" s="34"/>
-      <c r="J61" s="34"/>
-      <c r="K61" s="34"/>
-      <c r="L61" s="34"/>
-      <c r="M61" s="11"/>
+      <c r="B61" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F61" s="32"/>
+      <c r="H61" s="33"/>
+      <c r="I61" s="33"/>
+      <c r="J61" s="33"/>
+      <c r="K61" s="33"/>
+      <c r="L61" s="33"/>
+      <c r="M61" s="10"/>
     </row>
     <row r="62" spans="1:14" customHeight="1" ht="3.75">
-      <c r="B62" s="12"/>
-      <c r="F62" s="33"/>
-      <c r="M62" s="13"/>
+      <c r="B62" s="11"/>
+      <c r="F62" s="32"/>
+      <c r="M62" s="12"/>
     </row>
     <row r="63" spans="1:14" customHeight="1" ht="13.5">
-      <c r="B63" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="F63" s="33"/>
-      <c r="H63" s="34"/>
-      <c r="I63" s="34"/>
-      <c r="J63" s="34"/>
-      <c r="K63" s="34"/>
-      <c r="L63" s="34"/>
-      <c r="M63" s="11"/>
+      <c r="B63" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="F63" s="32"/>
+      <c r="H63" s="33"/>
+      <c r="I63" s="33"/>
+      <c r="J63" s="33"/>
+      <c r="K63" s="33"/>
+      <c r="L63" s="33"/>
+      <c r="M63" s="10"/>
     </row>
     <row r="64" spans="1:14" customHeight="1" ht="3.75">
-      <c r="B64" s="12"/>
-      <c r="F64" s="19"/>
-      <c r="M64" s="13"/>
+      <c r="B64" s="11"/>
+      <c r="F64" s="18"/>
+      <c r="M64" s="12"/>
     </row>
     <row r="65" spans="1:14" customHeight="1" ht="13.5">
-      <c r="B65" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="F65" s="33" t="s">
-        <v>6</v>
-      </c>
-      <c r="H65" s="34"/>
-      <c r="I65" s="34"/>
-      <c r="J65" s="34"/>
-      <c r="K65" s="34"/>
-      <c r="L65" s="34"/>
-      <c r="M65" s="11"/>
+      <c r="B65" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="F65" s="45" t="s">
+        <v>8</v>
+      </c>
+      <c r="H65" s="33"/>
+      <c r="I65" s="33"/>
+      <c r="J65" s="33"/>
+      <c r="K65" s="33"/>
+      <c r="L65" s="33"/>
+      <c r="M65" s="10"/>
     </row>
     <row r="66" spans="1:14" customHeight="1" ht="3.75">
-      <c r="B66" s="12"/>
-      <c r="F66" s="19"/>
-      <c r="M66" s="13"/>
+      <c r="B66" s="11"/>
+      <c r="F66" s="18"/>
+      <c r="M66" s="12"/>
     </row>
     <row r="67" spans="1:14" customHeight="1" ht="13.5">
-      <c r="B67" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="F67" s="33" t="s">
-        <v>6</v>
-      </c>
-      <c r="H67" s="34"/>
-      <c r="I67" s="34"/>
-      <c r="J67" s="34"/>
-      <c r="K67" s="34"/>
-      <c r="L67" s="34"/>
-      <c r="M67" s="11"/>
+      <c r="B67" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="F67" s="45" t="s">
+        <v>8</v>
+      </c>
+      <c r="H67" s="33"/>
+      <c r="I67" s="33"/>
+      <c r="J67" s="33"/>
+      <c r="K67" s="33"/>
+      <c r="L67" s="33"/>
+      <c r="M67" s="10"/>
     </row>
     <row r="68" spans="1:14" customHeight="1" ht="3.75">
-      <c r="B68" s="12"/>
-      <c r="M68" s="13"/>
+      <c r="B68" s="11"/>
+      <c r="M68" s="12"/>
     </row>
     <row r="69" spans="1:14">
-      <c r="B69" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="F69" s="34"/>
-      <c r="H69" s="34"/>
-      <c r="I69" s="34"/>
-      <c r="J69" s="34"/>
-      <c r="K69" s="34"/>
-      <c r="L69" s="34"/>
-      <c r="M69" s="11"/>
+      <c r="B69" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="F69" s="33"/>
+      <c r="H69" s="33"/>
+      <c r="I69" s="33"/>
+      <c r="J69" s="33"/>
+      <c r="K69" s="33"/>
+      <c r="L69" s="33"/>
+      <c r="M69" s="10"/>
     </row>
     <row r="70" spans="1:14" customHeight="1" ht="7.5">
-      <c r="B70" s="35"/>
-      <c r="C70" s="25"/>
-      <c r="D70" s="25"/>
-      <c r="E70" s="25"/>
-      <c r="F70" s="25"/>
-      <c r="G70" s="25"/>
-      <c r="H70" s="25"/>
-      <c r="I70" s="25"/>
-      <c r="J70" s="25"/>
-      <c r="K70" s="25"/>
-      <c r="L70" s="25"/>
-      <c r="M70" s="26"/>
+      <c r="B70" s="34"/>
+      <c r="C70" s="24"/>
+      <c r="D70" s="24"/>
+      <c r="E70" s="24"/>
+      <c r="F70" s="24"/>
+      <c r="G70" s="24"/>
+      <c r="H70" s="24"/>
+      <c r="I70" s="24"/>
+      <c r="J70" s="24"/>
+      <c r="K70" s="24"/>
+      <c r="L70" s="24"/>
+      <c r="M70" s="25"/>
     </row>
     <row r="71" spans="1:14" customHeight="1" ht="7.5"/>
     <row r="72" spans="1:14" customHeight="1" ht="7.5">
-      <c r="B72" s="20"/>
+      <c r="B72" s="19"/>
       <c r="C72" s="6"/>
       <c r="D72" s="6"/>
       <c r="E72" s="6"/>
@@ -1818,74 +1849,74 @@
       <c r="M72" s="7"/>
     </row>
     <row r="73" spans="1:14">
-      <c r="A73" s="19"/>
-      <c r="B73" s="51" t="s">
-        <v>52</v>
-      </c>
-      <c r="C73" s="52"/>
-      <c r="D73" s="19"/>
-      <c r="E73" s="19"/>
-      <c r="F73" s="52" t="s">
+      <c r="A73" s="18"/>
+      <c r="B73" s="54" t="s">
         <v>53</v>
       </c>
-      <c r="G73" s="52"/>
-      <c r="H73" s="52"/>
-      <c r="I73" s="52"/>
-      <c r="L73" s="52" t="s">
+      <c r="C73" s="48"/>
+      <c r="D73" s="18"/>
+      <c r="E73" s="18"/>
+      <c r="F73" s="48" t="s">
         <v>54</v>
       </c>
-      <c r="M73" s="53"/>
+      <c r="G73" s="48"/>
+      <c r="H73" s="48"/>
+      <c r="I73" s="48"/>
+      <c r="L73" s="48" t="s">
+        <v>55</v>
+      </c>
+      <c r="M73" s="49"/>
     </row>
     <row r="74" spans="1:14">
-      <c r="A74" s="19"/>
-      <c r="B74" s="60"/>
-      <c r="C74" s="59"/>
-      <c r="D74" s="19"/>
-      <c r="E74" s="19"/>
-      <c r="F74" s="19"/>
-      <c r="G74" s="19"/>
-      <c r="H74" s="19"/>
-      <c r="I74" s="19"/>
-      <c r="L74" s="19"/>
-      <c r="M74" s="42"/>
+      <c r="A74" s="18"/>
+      <c r="B74" s="57"/>
+      <c r="C74" s="58"/>
+      <c r="D74" s="18"/>
+      <c r="E74" s="18"/>
+      <c r="F74" s="18"/>
+      <c r="G74" s="18"/>
+      <c r="H74" s="18"/>
+      <c r="I74" s="18"/>
+      <c r="L74" s="18"/>
+      <c r="M74" s="41"/>
     </row>
     <row r="75" spans="1:14" customHeight="1" ht="12.75">
-      <c r="B75" s="61"/>
-      <c r="C75" s="58"/>
-      <c r="M75" s="13"/>
+      <c r="B75" s="43"/>
+      <c r="C75" s="42"/>
+      <c r="M75" s="12"/>
     </row>
     <row r="76" spans="1:14" customHeight="1" ht="33">
-      <c r="A76" s="19"/>
-      <c r="B76" s="57" t="s">
-        <v>11</v>
+      <c r="A76" s="18"/>
+      <c r="B76" s="55" t="s">
+        <v>12</v>
       </c>
       <c r="C76" s="56"/>
-      <c r="D76" s="19"/>
-      <c r="E76" s="19"/>
-      <c r="F76" s="45" t="s">
-        <v>55</v>
-      </c>
-      <c r="G76" s="45"/>
-      <c r="H76" s="45"/>
-      <c r="I76" s="45"/>
-      <c r="L76" s="45" t="s">
+      <c r="D76" s="18"/>
+      <c r="E76" s="18"/>
+      <c r="F76" s="50" t="s">
         <v>56</v>
       </c>
-      <c r="M76" s="46"/>
+      <c r="G76" s="50"/>
+      <c r="H76" s="50"/>
+      <c r="I76" s="50"/>
+      <c r="L76" s="50" t="s">
+        <v>57</v>
+      </c>
+      <c r="M76" s="51"/>
     </row>
     <row r="77" spans="1:14" customHeight="1" ht="8.25">
-      <c r="B77" s="35"/>
-      <c r="C77" s="25"/>
-      <c r="D77" s="25"/>
-      <c r="E77" s="25"/>
-      <c r="F77" s="25"/>
-      <c r="G77" s="25"/>
-      <c r="H77" s="25"/>
-      <c r="I77" s="25"/>
-      <c r="J77" s="25"/>
-      <c r="K77" s="25"/>
-      <c r="L77" s="25"/>
-      <c r="M77" s="26"/>
+      <c r="B77" s="34"/>
+      <c r="C77" s="24"/>
+      <c r="D77" s="24"/>
+      <c r="E77" s="24"/>
+      <c r="F77" s="24"/>
+      <c r="G77" s="24"/>
+      <c r="H77" s="24"/>
+      <c r="I77" s="24"/>
+      <c r="J77" s="24"/>
+      <c r="K77" s="24"/>
+      <c r="L77" s="24"/>
+      <c r="M77" s="25"/>
     </row>
     <row r="78" spans="1:14" customHeight="1" ht="5.25">
       <c r="M78" s="9"/>
@@ -1893,31 +1924,6 @@
     <row r="79" spans="1:14" customHeight="1" ht="15.75" hidden="true"/>
   </sheetData>
   <mergeCells>
-    <mergeCell ref="L73:M73"/>
-    <mergeCell ref="F76:I76"/>
-    <mergeCell ref="L76:M76"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="G35:I35"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="G37:I37"/>
-    <mergeCell ref="B73:C73"/>
-    <mergeCell ref="F73:I73"/>
-    <mergeCell ref="B76:C76"/>
-    <mergeCell ref="B74:C74"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="G33:I33"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="J21:M21"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="E23:M23"/>
-    <mergeCell ref="B27:F27"/>
-    <mergeCell ref="H27:M27"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="G29:I29"/>
-    <mergeCell ref="M29:M31"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="G31:I31"/>
     <mergeCell ref="B19:C19"/>
     <mergeCell ref="D19:F19"/>
     <mergeCell ref="H19:I19"/>
@@ -1934,6 +1940,31 @@
     <mergeCell ref="C17:F17"/>
     <mergeCell ref="H17:I17"/>
     <mergeCell ref="J17:M17"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="G33:I33"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="J21:M21"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="E23:M23"/>
+    <mergeCell ref="B27:F27"/>
+    <mergeCell ref="H27:M27"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="G29:I29"/>
+    <mergeCell ref="M29:M31"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="G31:I31"/>
+    <mergeCell ref="L73:M73"/>
+    <mergeCell ref="F76:I76"/>
+    <mergeCell ref="L76:M76"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="G35:I35"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="G37:I37"/>
+    <mergeCell ref="B73:C73"/>
+    <mergeCell ref="F73:I73"/>
+    <mergeCell ref="B76:C76"/>
+    <mergeCell ref="B74:C74"/>
   </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true" horizontalCentered="true"/>
   <pageMargins left="0.19685039370079" right="0.19685039370079" top="0" bottom="0" header="0" footer="0.19685039370079"/>

</xml_diff>

<commit_message>
se finaliza incrustracion de datos a excel
</commit_message>
<xml_diff>
--- a/imagenes_guardadas/archivo_con_firma.xlsx
+++ b/imagenes_guardadas/archivo_con_firma.xlsx
@@ -7,10 +7,10 @@
     <workbookView activeTab="0" autoFilterDateGrouping="true" firstSheet="0" minimized="false" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="Ángel Roberto Coronado" sheetId="1" r:id="rId4"/>
+    <sheet name="plantilla" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Ángel Roberto Coronado'!$B$1:$M$79</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'plantilla'!$B$1:$M$79</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="1" fullCalcOnLoad="0" forceFullCalc="0"/>
 </workbook>
@@ -28,24 +28,24 @@
     <t>Fecha de realización:</t>
   </si>
   <si>
-    <t>22/01/2025</t>
+    <t>02/01/2025</t>
   </si>
   <si>
     <t>No. de reporte:</t>
   </si>
   <si>
-    <t>PM15012025</t>
+    <t>PM02012025</t>
   </si>
   <si>
     <t>Programado</t>
   </si>
   <si>
+    <t>✓</t>
+  </si>
+  <si>
     <t>Solicitado</t>
   </si>
   <si>
-    <t>✓</t>
-  </si>
-  <si>
     <t>Observación:</t>
   </si>
   <si>
@@ -61,19 +61,19 @@
     <t>Puesto:</t>
   </si>
   <si>
-    <t>Administrador de Egresos</t>
+    <t>AUXLIAR</t>
   </si>
   <si>
     <t>No. de serie:</t>
   </si>
   <si>
-    <t>3719351401462</t>
+    <t>22526DDDD</t>
   </si>
   <si>
     <t>Capacidad de disco:</t>
   </si>
   <si>
-    <t>500GB NVMe</t>
+    <t>55GB</t>
   </si>
   <si>
     <t>No. de inventario:</t>
@@ -82,7 +82,7 @@
     <t>Capacidad de memoria:</t>
   </si>
   <si>
-    <t>8GB</t>
+    <t>66GB</t>
   </si>
   <si>
     <t>Espacio disponible:</t>
@@ -263,7 +263,7 @@
       <name val="CorpoS"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -273,12 +273,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
@@ -427,7 +421,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="67">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
     <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0"/>
     <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0"/>
@@ -522,39 +516,63 @@
     <xf xfId="0" fontId="6" numFmtId="0" fillId="2" borderId="4" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
     </xf>
+    <xf xfId="0" fontId="1" numFmtId="14" fillId="3" borderId="11" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="0"/>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="3" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0"/>
     <xf xfId="0" fontId="5" numFmtId="0" fillId="3" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="1">
       <alignment vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="5" numFmtId="0" fillId="3" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="1" numFmtId="14" fillId="4" borderId="11" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="0"/>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="4" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0"/>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="4" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="3" borderId="11" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="11" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="5" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="4" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="3" borderId="5" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="49" fillId="3" borderId="11" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="49" fillId="3" borderId="5" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="4" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
     <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="6" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="11" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="5" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="4" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="4" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="6" numFmtId="0" fillId="4" borderId="12" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="6" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="6" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="6" numFmtId="0" fillId="3" borderId="12" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="6" numFmtId="0" fillId="4" borderId="11" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="6" numFmtId="0" fillId="3" borderId="11" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="6" numFmtId="0" fillId="2" borderId="4" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -562,36 +580,6 @@
     </xf>
     <xf xfId="0" fontId="6" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="4" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="3" borderId="11" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="6" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="6" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="3" borderId="5" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="4" borderId="11" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="4" borderId="5" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="49" fillId="3" borderId="11" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="49" fillId="3" borderId="5" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -648,7 +636,7 @@
       <xdr:row>73</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="1019175" cy="514350"/>
+    <xdr:ext cx="1009650" cy="514350"/>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="2" name="Firma" descr="Firma digital"/>
@@ -1000,8 +988,8 @@
   </sheetPr>
   <dimension ref="A1:N79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" view="pageBreakPreview" showGridLines="true" showRowColHeaders="1" topLeftCell="A65">
-      <selection activeCell="B76" sqref="B76:C76"/>
+    <sheetView tabSelected="1" workbookViewId="0" view="pageBreakPreview" showGridLines="true" showRowColHeaders="1" topLeftCell="A2">
+      <selection activeCell="L7" sqref="L7:M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1053,25 +1041,25 @@
       <c r="M6" s="7"/>
     </row>
     <row r="7" spans="1:14">
-      <c r="B7" s="52" t="s">
+      <c r="B7" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="53"/>
-      <c r="D7" s="53"/>
-      <c r="E7" s="53"/>
-      <c r="F7" s="46" t="s">
+      <c r="C7" s="54"/>
+      <c r="D7" s="54"/>
+      <c r="E7" s="54"/>
+      <c r="F7" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="H7" s="53" t="s">
+      <c r="H7" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="I7" s="53"/>
-      <c r="J7" s="53"/>
-      <c r="K7" s="53"/>
-      <c r="L7" s="61" t="s">
+      <c r="I7" s="54"/>
+      <c r="J7" s="54"/>
+      <c r="K7" s="54"/>
+      <c r="L7" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="M7" s="64"/>
+      <c r="M7" s="55"/>
     </row>
     <row r="8" spans="1:14" customHeight="1" ht="7.5">
       <c r="B8" s="11"/>
@@ -1079,20 +1067,20 @@
     </row>
     <row r="9" spans="1:14" customHeight="1" ht="13.5">
       <c r="A9" s="9"/>
-      <c r="B9" s="52" t="s">
+      <c r="B9" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="53"/>
-      <c r="D9" s="47"/>
+      <c r="C9" s="54"/>
+      <c r="D9" s="45" t="s">
+        <v>7</v>
+      </c>
       <c r="F9" s="9"/>
       <c r="G9" s="9"/>
-      <c r="H9" s="53" t="s">
-        <v>7</v>
-      </c>
-      <c r="I9" s="53"/>
-      <c r="J9" s="47" t="s">
+      <c r="H9" s="54" t="s">
         <v>8</v>
       </c>
+      <c r="I9" s="54"/>
+      <c r="J9" s="45"/>
       <c r="K9" s="13"/>
       <c r="L9" s="9"/>
       <c r="M9" s="14"/>
@@ -1114,22 +1102,22 @@
     </row>
     <row r="11" spans="1:14">
       <c r="A11" s="9"/>
-      <c r="B11" s="52" t="s">
+      <c r="B11" s="53" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="53"/>
+      <c r="C11" s="54"/>
       <c r="D11" s="9"/>
-      <c r="E11" s="65" t="s">
+      <c r="E11" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="F11" s="65"/>
-      <c r="G11" s="65"/>
-      <c r="H11" s="65"/>
-      <c r="I11" s="65"/>
-      <c r="J11" s="65"/>
-      <c r="K11" s="65"/>
-      <c r="L11" s="65"/>
-      <c r="M11" s="66"/>
+      <c r="F11" s="50"/>
+      <c r="G11" s="50"/>
+      <c r="H11" s="50"/>
+      <c r="I11" s="50"/>
+      <c r="J11" s="50"/>
+      <c r="K11" s="50"/>
+      <c r="L11" s="50"/>
+      <c r="M11" s="55"/>
     </row>
     <row r="12" spans="1:14" customHeight="1" ht="7.5">
       <c r="A12" s="9"/>
@@ -1177,22 +1165,22 @@
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="9"/>
-      <c r="B15" s="59" t="s">
+      <c r="B15" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="60"/>
+      <c r="C15" s="49"/>
       <c r="D15" s="21"/>
       <c r="E15" s="9"/>
-      <c r="F15" s="65" t="s">
+      <c r="F15" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="G15" s="65"/>
-      <c r="H15" s="65"/>
-      <c r="I15" s="65"/>
-      <c r="J15" s="65"/>
-      <c r="K15" s="65"/>
-      <c r="L15" s="65"/>
-      <c r="M15" s="66"/>
+      <c r="G15" s="50"/>
+      <c r="H15" s="50"/>
+      <c r="I15" s="50"/>
+      <c r="J15" s="50"/>
+      <c r="K15" s="50"/>
+      <c r="L15" s="50"/>
+      <c r="M15" s="55"/>
     </row>
     <row r="16" spans="1:14" customHeight="1" ht="7.5">
       <c r="B16" s="11"/>
@@ -1202,22 +1190,22 @@
       <c r="B17" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="61" t="s">
+      <c r="C17" s="50" t="s">
         <v>14</v>
       </c>
-      <c r="D17" s="61"/>
-      <c r="E17" s="61"/>
-      <c r="F17" s="61"/>
-      <c r="H17" s="60" t="s">
+      <c r="D17" s="50"/>
+      <c r="E17" s="50"/>
+      <c r="F17" s="50"/>
+      <c r="H17" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="I17" s="60"/>
-      <c r="J17" s="67" t="s">
+      <c r="I17" s="49"/>
+      <c r="J17" s="56" t="s">
         <v>16</v>
       </c>
-      <c r="K17" s="67"/>
-      <c r="L17" s="67"/>
-      <c r="M17" s="68"/>
+      <c r="K17" s="56"/>
+      <c r="L17" s="56"/>
+      <c r="M17" s="57"/>
     </row>
     <row r="18" spans="1:14" customHeight="1" ht="7.5">
       <c r="B18" s="11"/>
@@ -1225,23 +1213,23 @@
     </row>
     <row r="19" spans="1:14">
       <c r="A19" s="9"/>
-      <c r="B19" s="59" t="s">
+      <c r="B19" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="60"/>
-      <c r="D19" s="61" t="s">
+      <c r="C19" s="49"/>
+      <c r="D19" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="E19" s="61"/>
-      <c r="F19" s="61"/>
-      <c r="H19" s="60" t="s">
+      <c r="E19" s="50"/>
+      <c r="F19" s="50"/>
+      <c r="H19" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="I19" s="60"/>
-      <c r="J19" s="50"/>
-      <c r="K19" s="50"/>
-      <c r="L19" s="50"/>
-      <c r="M19" s="51"/>
+      <c r="I19" s="49"/>
+      <c r="J19" s="51"/>
+      <c r="K19" s="51"/>
+      <c r="L19" s="51"/>
+      <c r="M19" s="52"/>
     </row>
     <row r="20" spans="1:14" customHeight="1" ht="7.5">
       <c r="B20" s="11"/>
@@ -1249,23 +1237,23 @@
     </row>
     <row r="21" spans="1:14">
       <c r="A21" s="9"/>
-      <c r="B21" s="59" t="s">
+      <c r="B21" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="60"/>
-      <c r="D21" s="61" t="s">
+      <c r="C21" s="49"/>
+      <c r="D21" s="50" t="s">
         <v>21</v>
       </c>
-      <c r="E21" s="61"/>
-      <c r="F21" s="61"/>
+      <c r="E21" s="50"/>
+      <c r="F21" s="50"/>
       <c r="H21" s="21" t="s">
         <v>22</v>
       </c>
       <c r="I21" s="21"/>
-      <c r="J21" s="50"/>
-      <c r="K21" s="50"/>
-      <c r="L21" s="50"/>
-      <c r="M21" s="51"/>
+      <c r="J21" s="51"/>
+      <c r="K21" s="51"/>
+      <c r="L21" s="51"/>
+      <c r="M21" s="52"/>
     </row>
     <row r="22" spans="1:14" customHeight="1" ht="7.5">
       <c r="B22" s="11"/>
@@ -1273,22 +1261,22 @@
     </row>
     <row r="23" spans="1:14">
       <c r="A23" s="9"/>
-      <c r="B23" s="52" t="s">
+      <c r="B23" s="53" t="s">
         <v>9</v>
       </c>
-      <c r="C23" s="53"/>
+      <c r="C23" s="54"/>
       <c r="D23" s="9"/>
-      <c r="E23" s="50" t="s">
+      <c r="E23" s="51" t="s">
         <v>23</v>
       </c>
-      <c r="F23" s="50"/>
-      <c r="G23" s="50"/>
-      <c r="H23" s="50"/>
-      <c r="I23" s="50"/>
-      <c r="J23" s="50"/>
-      <c r="K23" s="50"/>
-      <c r="L23" s="50"/>
-      <c r="M23" s="51"/>
+      <c r="F23" s="51"/>
+      <c r="G23" s="51"/>
+      <c r="H23" s="51"/>
+      <c r="I23" s="51"/>
+      <c r="J23" s="51"/>
+      <c r="K23" s="51"/>
+      <c r="L23" s="51"/>
+      <c r="M23" s="52"/>
     </row>
     <row r="24" spans="1:14" customHeight="1" ht="7.5">
       <c r="A24" s="9"/>
@@ -1328,21 +1316,21 @@
       <c r="M26" s="7"/>
     </row>
     <row r="27" spans="1:14">
-      <c r="B27" s="54" t="s">
+      <c r="B27" s="58" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="48"/>
-      <c r="D27" s="48"/>
-      <c r="E27" s="48"/>
-      <c r="F27" s="48"/>
-      <c r="H27" s="48" t="s">
+      <c r="C27" s="59"/>
+      <c r="D27" s="59"/>
+      <c r="E27" s="59"/>
+      <c r="F27" s="59"/>
+      <c r="H27" s="59" t="s">
         <v>25</v>
       </c>
-      <c r="I27" s="48"/>
-      <c r="J27" s="48"/>
-      <c r="K27" s="48"/>
-      <c r="L27" s="48"/>
-      <c r="M27" s="49"/>
+      <c r="I27" s="59"/>
+      <c r="J27" s="59"/>
+      <c r="K27" s="59"/>
+      <c r="L27" s="59"/>
+      <c r="M27" s="60"/>
     </row>
     <row r="28" spans="1:14" customHeight="1" ht="7.5">
       <c r="A28" s="9"/>
@@ -1354,24 +1342,26 @@
     </row>
     <row r="29" spans="1:14" customHeight="1" ht="13.5">
       <c r="A29" s="9"/>
-      <c r="B29" s="52" t="s">
+      <c r="B29" s="53" t="s">
         <v>26</v>
       </c>
-      <c r="C29" s="53"/>
+      <c r="C29" s="54"/>
       <c r="D29" s="9"/>
-      <c r="E29" s="44"/>
+      <c r="E29" s="46" t="s">
+        <v>7</v>
+      </c>
       <c r="F29" s="9"/>
-      <c r="G29" s="53" t="s">
+      <c r="G29" s="54" t="s">
         <v>27</v>
       </c>
-      <c r="H29" s="53"/>
-      <c r="I29" s="53"/>
+      <c r="H29" s="54"/>
+      <c r="I29" s="54"/>
       <c r="J29" s="9"/>
       <c r="K29" s="13"/>
-      <c r="L29" s="44" t="s">
-        <v>8</v>
-      </c>
-      <c r="M29" s="62"/>
+      <c r="L29" s="46" t="s">
+        <v>7</v>
+      </c>
+      <c r="M29" s="61"/>
     </row>
     <row r="30" spans="1:14" customHeight="1" ht="7.5">
       <c r="B30" s="28"/>
@@ -1382,28 +1372,30 @@
       <c r="J30" s="9"/>
       <c r="K30" s="9"/>
       <c r="L30" s="9"/>
-      <c r="M30" s="63"/>
+      <c r="M30" s="62"/>
     </row>
     <row r="31" spans="1:14" customHeight="1" ht="13.5">
       <c r="A31" s="9"/>
-      <c r="B31" s="52" t="s">
+      <c r="B31" s="53" t="s">
         <v>28</v>
       </c>
-      <c r="C31" s="53"/>
+      <c r="C31" s="54"/>
       <c r="D31" s="9"/>
-      <c r="E31" s="44"/>
+      <c r="E31" s="46" t="s">
+        <v>7</v>
+      </c>
       <c r="F31" s="9"/>
-      <c r="G31" s="53" t="s">
+      <c r="G31" s="54" t="s">
         <v>29</v>
       </c>
-      <c r="H31" s="53"/>
-      <c r="I31" s="53"/>
+      <c r="H31" s="54"/>
+      <c r="I31" s="54"/>
       <c r="J31" s="9"/>
       <c r="K31" s="13"/>
-      <c r="L31" s="44" t="s">
-        <v>8</v>
-      </c>
-      <c r="M31" s="63"/>
+      <c r="L31" s="46" t="s">
+        <v>7</v>
+      </c>
+      <c r="M31" s="62"/>
     </row>
     <row r="32" spans="1:14" customHeight="1" ht="7.5">
       <c r="B32" s="8"/>
@@ -1418,20 +1410,20 @@
     </row>
     <row r="33" spans="1:14" customHeight="1" ht="13.5">
       <c r="A33" s="9"/>
-      <c r="B33" s="52" t="s">
+      <c r="B33" s="53" t="s">
         <v>30</v>
       </c>
-      <c r="C33" s="53"/>
+      <c r="C33" s="54"/>
       <c r="D33" s="9"/>
-      <c r="E33" s="44" t="s">
-        <v>8</v>
+      <c r="E33" s="46" t="s">
+        <v>7</v>
       </c>
       <c r="F33" s="9"/>
-      <c r="G33" s="53" t="s">
+      <c r="G33" s="54" t="s">
         <v>31</v>
       </c>
-      <c r="H33" s="53"/>
-      <c r="I33" s="53"/>
+      <c r="H33" s="54"/>
+      <c r="I33" s="54"/>
       <c r="J33" s="9"/>
       <c r="K33" s="29"/>
       <c r="L33" s="9"/>
@@ -1450,17 +1442,19 @@
     </row>
     <row r="35" spans="1:14" customHeight="1" ht="13.5">
       <c r="A35" s="9"/>
-      <c r="B35" s="52" t="s">
+      <c r="B35" s="53" t="s">
         <v>32</v>
       </c>
-      <c r="C35" s="53"/>
+      <c r="C35" s="54"/>
       <c r="D35" s="9"/>
-      <c r="E35" s="13"/>
-      <c r="G35" s="53" t="s">
+      <c r="E35" s="46" t="s">
+        <v>7</v>
+      </c>
+      <c r="G35" s="54" t="s">
         <v>33</v>
       </c>
-      <c r="H35" s="53"/>
-      <c r="I35" s="53"/>
+      <c r="H35" s="54"/>
+      <c r="I35" s="54"/>
       <c r="J35" s="9"/>
       <c r="K35" s="29"/>
       <c r="L35" s="9"/>
@@ -1479,18 +1473,20 @@
     </row>
     <row r="37" spans="1:14" customHeight="1" ht="13.5">
       <c r="A37" s="9"/>
-      <c r="B37" s="52" t="s">
+      <c r="B37" s="53" t="s">
         <v>34</v>
       </c>
-      <c r="C37" s="53"/>
+      <c r="C37" s="54"/>
       <c r="D37" s="9"/>
-      <c r="E37" s="13"/>
+      <c r="E37" s="46" t="s">
+        <v>7</v>
+      </c>
       <c r="F37" s="18"/>
-      <c r="G37" s="53" t="s">
+      <c r="G37" s="54" t="s">
         <v>35</v>
       </c>
-      <c r="H37" s="53"/>
-      <c r="I37" s="53"/>
+      <c r="H37" s="54"/>
+      <c r="I37" s="54"/>
       <c r="J37" s="9"/>
       <c r="K37" s="29"/>
       <c r="L37" s="18"/>
@@ -1560,8 +1556,8 @@
       <c r="B43" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="F43" s="45" t="s">
-        <v>8</v>
+      <c r="F43" s="47" t="s">
+        <v>7</v>
       </c>
       <c r="H43" s="33"/>
       <c r="I43" s="33"/>
@@ -1578,8 +1574,8 @@
       <c r="B45" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="F45" s="45" t="s">
-        <v>8</v>
+      <c r="F45" s="47" t="s">
+        <v>7</v>
       </c>
       <c r="H45" s="33"/>
       <c r="I45" s="33"/>
@@ -1596,8 +1592,8 @@
       <c r="B47" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="F47" s="45" t="s">
-        <v>8</v>
+      <c r="F47" s="47" t="s">
+        <v>7</v>
       </c>
       <c r="H47" s="33"/>
       <c r="I47" s="33"/>
@@ -1614,8 +1610,8 @@
       <c r="B49" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="F49" s="45" t="s">
-        <v>8</v>
+      <c r="F49" s="47" t="s">
+        <v>7</v>
       </c>
       <c r="H49" s="33"/>
       <c r="I49" s="33"/>
@@ -1632,8 +1628,8 @@
       <c r="B51" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="F51" s="45" t="s">
-        <v>8</v>
+      <c r="F51" s="47" t="s">
+        <v>7</v>
       </c>
       <c r="H51" s="33"/>
       <c r="I51" s="33"/>
@@ -1702,8 +1698,8 @@
       <c r="B57" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="F57" s="45" t="s">
-        <v>8</v>
+      <c r="F57" s="47" t="s">
+        <v>7</v>
       </c>
       <c r="H57" s="33"/>
       <c r="I57" s="33"/>
@@ -1721,8 +1717,8 @@
       <c r="B59" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="F59" s="45" t="s">
-        <v>8</v>
+      <c r="F59" s="47" t="s">
+        <v>7</v>
       </c>
       <c r="H59" s="33"/>
       <c r="I59" s="33"/>
@@ -1740,7 +1736,9 @@
       <c r="B61" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="F61" s="32"/>
+      <c r="F61" s="47" t="s">
+        <v>7</v>
+      </c>
       <c r="H61" s="33"/>
       <c r="I61" s="33"/>
       <c r="J61" s="33"/>
@@ -1757,7 +1755,9 @@
       <c r="B63" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="F63" s="32"/>
+      <c r="F63" s="47" t="s">
+        <v>7</v>
+      </c>
       <c r="H63" s="33"/>
       <c r="I63" s="33"/>
       <c r="J63" s="33"/>
@@ -1774,8 +1774,8 @@
       <c r="B65" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="F65" s="45" t="s">
-        <v>8</v>
+      <c r="F65" s="47" t="s">
+        <v>7</v>
       </c>
       <c r="H65" s="33"/>
       <c r="I65" s="33"/>
@@ -1793,8 +1793,8 @@
       <c r="B67" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="F67" s="45" t="s">
-        <v>8</v>
+      <c r="F67" s="47" t="s">
+        <v>7</v>
       </c>
       <c r="H67" s="33"/>
       <c r="I67" s="33"/>
@@ -1850,27 +1850,27 @@
     </row>
     <row r="73" spans="1:14">
       <c r="A73" s="18"/>
-      <c r="B73" s="54" t="s">
+      <c r="B73" s="58" t="s">
         <v>53</v>
       </c>
-      <c r="C73" s="48"/>
+      <c r="C73" s="59"/>
       <c r="D73" s="18"/>
       <c r="E73" s="18"/>
-      <c r="F73" s="48" t="s">
+      <c r="F73" s="59" t="s">
         <v>54</v>
       </c>
-      <c r="G73" s="48"/>
-      <c r="H73" s="48"/>
-      <c r="I73" s="48"/>
-      <c r="L73" s="48" t="s">
+      <c r="G73" s="59"/>
+      <c r="H73" s="59"/>
+      <c r="I73" s="59"/>
+      <c r="L73" s="59" t="s">
         <v>55</v>
       </c>
-      <c r="M73" s="49"/>
+      <c r="M73" s="60"/>
     </row>
     <row r="74" spans="1:14">
       <c r="A74" s="18"/>
-      <c r="B74" s="57"/>
-      <c r="C74" s="58"/>
+      <c r="B74" s="65"/>
+      <c r="C74" s="66"/>
       <c r="D74" s="18"/>
       <c r="E74" s="18"/>
       <c r="F74" s="18"/>
@@ -1887,22 +1887,22 @@
     </row>
     <row r="76" spans="1:14" customHeight="1" ht="33">
       <c r="A76" s="18"/>
-      <c r="B76" s="55" t="s">
+      <c r="B76" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="C76" s="56"/>
+      <c r="C76" s="64"/>
       <c r="D76" s="18"/>
       <c r="E76" s="18"/>
-      <c r="F76" s="50" t="s">
+      <c r="F76" s="51" t="s">
         <v>56</v>
       </c>
-      <c r="G76" s="50"/>
-      <c r="H76" s="50"/>
-      <c r="I76" s="50"/>
-      <c r="L76" s="50" t="s">
+      <c r="G76" s="51"/>
+      <c r="H76" s="51"/>
+      <c r="I76" s="51"/>
+      <c r="L76" s="51" t="s">
         <v>57</v>
       </c>
-      <c r="M76" s="51"/>
+      <c r="M76" s="52"/>
     </row>
     <row r="77" spans="1:14" customHeight="1" ht="8.25">
       <c r="B77" s="34"/>
@@ -1924,6 +1924,31 @@
     <row r="79" spans="1:14" customHeight="1" ht="15.75" hidden="true"/>
   </sheetData>
   <mergeCells>
+    <mergeCell ref="L73:M73"/>
+    <mergeCell ref="F76:I76"/>
+    <mergeCell ref="L76:M76"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="G35:I35"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="G37:I37"/>
+    <mergeCell ref="B73:C73"/>
+    <mergeCell ref="F73:I73"/>
+    <mergeCell ref="B76:C76"/>
+    <mergeCell ref="B74:C74"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="G33:I33"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="J21:M21"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="E23:M23"/>
+    <mergeCell ref="B27:F27"/>
+    <mergeCell ref="H27:M27"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="G29:I29"/>
+    <mergeCell ref="M29:M31"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="G31:I31"/>
     <mergeCell ref="B19:C19"/>
     <mergeCell ref="D19:F19"/>
     <mergeCell ref="H19:I19"/>
@@ -1940,31 +1965,6 @@
     <mergeCell ref="C17:F17"/>
     <mergeCell ref="H17:I17"/>
     <mergeCell ref="J17:M17"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="G33:I33"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="J21:M21"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="E23:M23"/>
-    <mergeCell ref="B27:F27"/>
-    <mergeCell ref="H27:M27"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="G29:I29"/>
-    <mergeCell ref="M29:M31"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="G31:I31"/>
-    <mergeCell ref="L73:M73"/>
-    <mergeCell ref="F76:I76"/>
-    <mergeCell ref="L76:M76"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="G35:I35"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="G37:I37"/>
-    <mergeCell ref="B73:C73"/>
-    <mergeCell ref="F73:I73"/>
-    <mergeCell ref="B76:C76"/>
-    <mergeCell ref="B74:C74"/>
   </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true" horizontalCentered="true"/>
   <pageMargins left="0.19685039370079" right="0.19685039370079" top="0" bottom="0" header="0" footer="0.19685039370079"/>

</xml_diff>

<commit_message>
Wip: se crea modulo para tipo cards para mant y resg
</commit_message>
<xml_diff>
--- a/imagenes_guardadas/archivo_con_firma.xlsx
+++ b/imagenes_guardadas/archivo_con_firma.xlsx
@@ -28,24 +28,24 @@
     <t>Fecha de realización:</t>
   </si>
   <si>
-    <t>02/01/2025</t>
+    <t>24/02/2025</t>
   </si>
   <si>
     <t>No. de reporte:</t>
   </si>
   <si>
-    <t>PM02012025</t>
+    <t>PM24022025</t>
   </si>
   <si>
     <t>Programado</t>
   </si>
   <si>
+    <t>Solicitado</t>
+  </si>
+  <si>
     <t>✓</t>
   </si>
   <si>
-    <t>Solicitado</t>
-  </si>
-  <si>
     <t>Observación:</t>
   </si>
   <si>
@@ -55,25 +55,25 @@
     <t>Nombre del usuario:</t>
   </si>
   <si>
-    <t>Ana Karen Sevilla Pulido</t>
+    <t>Jose Maduro Moreno Leonardo</t>
   </si>
   <si>
     <t>Puesto:</t>
   </si>
   <si>
-    <t>AUXLIAR</t>
+    <t xml:space="preserve">Administración </t>
   </si>
   <si>
     <t>No. de serie:</t>
   </si>
   <si>
-    <t>22526DDDD</t>
+    <t>TYUHHRF</t>
   </si>
   <si>
     <t>Capacidad de disco:</t>
   </si>
   <si>
-    <t>55GB</t>
+    <t>150GB</t>
   </si>
   <si>
     <t>No. de inventario:</t>
@@ -82,7 +82,7 @@
     <t>Capacidad de memoria:</t>
   </si>
   <si>
-    <t>66GB</t>
+    <t>1501GB</t>
   </si>
   <si>
     <t>Espacio disponible:</t>
@@ -636,7 +636,7 @@
       <xdr:row>73</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="1009650" cy="514350"/>
+    <xdr:ext cx="1019175" cy="514350"/>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="2" name="Firma" descr="Firma digital"/>
@@ -1071,16 +1071,16 @@
         <v>6</v>
       </c>
       <c r="C9" s="54"/>
-      <c r="D9" s="45" t="s">
-        <v>7</v>
-      </c>
+      <c r="D9" s="45"/>
       <c r="F9" s="9"/>
       <c r="G9" s="9"/>
       <c r="H9" s="54" t="s">
+        <v>7</v>
+      </c>
+      <c r="I9" s="54"/>
+      <c r="J9" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="I9" s="54"/>
-      <c r="J9" s="45"/>
       <c r="K9" s="13"/>
       <c r="L9" s="9"/>
       <c r="M9" s="14"/>
@@ -1348,7 +1348,7 @@
       <c r="C29" s="54"/>
       <c r="D29" s="9"/>
       <c r="E29" s="46" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F29" s="9"/>
       <c r="G29" s="54" t="s">
@@ -1359,7 +1359,7 @@
       <c r="J29" s="9"/>
       <c r="K29" s="13"/>
       <c r="L29" s="46" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="M29" s="61"/>
     </row>
@@ -1382,7 +1382,7 @@
       <c r="C31" s="54"/>
       <c r="D31" s="9"/>
       <c r="E31" s="46" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F31" s="9"/>
       <c r="G31" s="54" t="s">
@@ -1393,7 +1393,7 @@
       <c r="J31" s="9"/>
       <c r="K31" s="13"/>
       <c r="L31" s="46" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="M31" s="62"/>
     </row>
@@ -1416,7 +1416,7 @@
       <c r="C33" s="54"/>
       <c r="D33" s="9"/>
       <c r="E33" s="46" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F33" s="9"/>
       <c r="G33" s="54" t="s">
@@ -1448,7 +1448,7 @@
       <c r="C35" s="54"/>
       <c r="D35" s="9"/>
       <c r="E35" s="46" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G35" s="54" t="s">
         <v>33</v>
@@ -1479,7 +1479,7 @@
       <c r="C37" s="54"/>
       <c r="D37" s="9"/>
       <c r="E37" s="46" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F37" s="18"/>
       <c r="G37" s="54" t="s">
@@ -1557,7 +1557,7 @@
         <v>39</v>
       </c>
       <c r="F43" s="47" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H43" s="33"/>
       <c r="I43" s="33"/>
@@ -1575,7 +1575,7 @@
         <v>40</v>
       </c>
       <c r="F45" s="47" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H45" s="33"/>
       <c r="I45" s="33"/>
@@ -1593,7 +1593,7 @@
         <v>41</v>
       </c>
       <c r="F47" s="47" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H47" s="33"/>
       <c r="I47" s="33"/>
@@ -1611,7 +1611,7 @@
         <v>42</v>
       </c>
       <c r="F49" s="47" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H49" s="33"/>
       <c r="I49" s="33"/>
@@ -1629,7 +1629,7 @@
         <v>43</v>
       </c>
       <c r="F51" s="47" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H51" s="33"/>
       <c r="I51" s="33"/>
@@ -1699,7 +1699,7 @@
         <v>46</v>
       </c>
       <c r="F57" s="47" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H57" s="33"/>
       <c r="I57" s="33"/>
@@ -1718,7 +1718,7 @@
         <v>47</v>
       </c>
       <c r="F59" s="47" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H59" s="33"/>
       <c r="I59" s="33"/>
@@ -1737,7 +1737,7 @@
         <v>48</v>
       </c>
       <c r="F61" s="47" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H61" s="33"/>
       <c r="I61" s="33"/>
@@ -1756,7 +1756,7 @@
         <v>49</v>
       </c>
       <c r="F63" s="47" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H63" s="33"/>
       <c r="I63" s="33"/>
@@ -1775,7 +1775,7 @@
         <v>50</v>
       </c>
       <c r="F65" s="47" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H65" s="33"/>
       <c r="I65" s="33"/>
@@ -1794,7 +1794,7 @@
         <v>51</v>
       </c>
       <c r="F67" s="47" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H67" s="33"/>
       <c r="I67" s="33"/>

</xml_diff>

<commit_message>
Se crea formato resguardo
</commit_message>
<xml_diff>
--- a/imagenes_guardadas/archivo_con_firma.xlsx
+++ b/imagenes_guardadas/archivo_con_firma.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="59">
   <si>
     <t>Automóviles y Camiones Rivera, S.A. de C.V.</t>
   </si>
@@ -28,24 +28,24 @@
     <t>Fecha de realización:</t>
   </si>
   <si>
-    <t>24/02/2025</t>
+    <t>27/01/2025</t>
   </si>
   <si>
     <t>No. de reporte:</t>
   </si>
   <si>
-    <t>PM24022025</t>
+    <t>PM27012025</t>
   </si>
   <si>
     <t>Programado</t>
   </si>
   <si>
+    <t>✓</t>
+  </si>
+  <si>
     <t>Solicitado</t>
   </si>
   <si>
-    <t>✓</t>
-  </si>
-  <si>
     <t>Observación:</t>
   </si>
   <si>
@@ -55,25 +55,25 @@
     <t>Nombre del usuario:</t>
   </si>
   <si>
-    <t>Jose Maduro Moreno Leonardo</t>
+    <t>Pedro Perico Hernandez</t>
   </si>
   <si>
     <t>Puesto:</t>
   </si>
   <si>
-    <t xml:space="preserve">Administración </t>
+    <t>AUXLIAR</t>
   </si>
   <si>
     <t>No. de serie:</t>
   </si>
   <si>
-    <t>TYUHHRF</t>
+    <t>22526DDDD</t>
   </si>
   <si>
     <t>Capacidad de disco:</t>
   </si>
   <si>
-    <t>150GB</t>
+    <t>855GB</t>
   </si>
   <si>
     <t>No. de inventario:</t>
@@ -82,7 +82,7 @@
     <t>Capacidad de memoria:</t>
   </si>
   <si>
-    <t>1501GB</t>
+    <t>555GB</t>
   </si>
   <si>
     <t>Espacio disponible:</t>
@@ -110,6 +110,9 @@
   </si>
   <si>
     <t>Interior / Exterior gabinete</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t>Borrar Archivos infectados</t>
@@ -636,7 +639,7 @@
       <xdr:row>73</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="1019175" cy="514350"/>
+    <xdr:ext cx="1009650" cy="514350"/>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="2" name="Firma" descr="Firma digital"/>
@@ -1071,16 +1074,16 @@
         <v>6</v>
       </c>
       <c r="C9" s="54"/>
-      <c r="D9" s="45"/>
+      <c r="D9" s="45" t="s">
+        <v>7</v>
+      </c>
       <c r="F9" s="9"/>
       <c r="G9" s="9"/>
       <c r="H9" s="54" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I9" s="54"/>
-      <c r="J9" s="45" t="s">
-        <v>8</v>
-      </c>
+      <c r="J9" s="45"/>
       <c r="K9" s="13"/>
       <c r="L9" s="9"/>
       <c r="M9" s="14"/>
@@ -1348,7 +1351,7 @@
       <c r="C29" s="54"/>
       <c r="D29" s="9"/>
       <c r="E29" s="46" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F29" s="9"/>
       <c r="G29" s="54" t="s">
@@ -1359,7 +1362,7 @@
       <c r="J29" s="9"/>
       <c r="K29" s="13"/>
       <c r="L29" s="46" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="M29" s="61"/>
     </row>
@@ -1382,7 +1385,7 @@
       <c r="C31" s="54"/>
       <c r="D31" s="9"/>
       <c r="E31" s="46" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F31" s="9"/>
       <c r="G31" s="54" t="s">
@@ -1393,7 +1396,7 @@
       <c r="J31" s="9"/>
       <c r="K31" s="13"/>
       <c r="L31" s="46" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="M31" s="62"/>
     </row>
@@ -1416,11 +1419,11 @@
       <c r="C33" s="54"/>
       <c r="D33" s="9"/>
       <c r="E33" s="46" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="F33" s="9"/>
       <c r="G33" s="54" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H33" s="54"/>
       <c r="I33" s="54"/>
@@ -1443,15 +1446,15 @@
     <row r="35" spans="1:14" customHeight="1" ht="13.5">
       <c r="A35" s="9"/>
       <c r="B35" s="53" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C35" s="54"/>
       <c r="D35" s="9"/>
       <c r="E35" s="46" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G35" s="54" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H35" s="54"/>
       <c r="I35" s="54"/>
@@ -1474,16 +1477,16 @@
     <row r="37" spans="1:14" customHeight="1" ht="13.5">
       <c r="A37" s="9"/>
       <c r="B37" s="53" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C37" s="54"/>
       <c r="D37" s="9"/>
       <c r="E37" s="46" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F37" s="18"/>
       <c r="G37" s="54" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H37" s="54"/>
       <c r="I37" s="54"/>
@@ -1538,26 +1541,26 @@
     </row>
     <row r="41" spans="1:14">
       <c r="B41" s="11" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="M41" s="12"/>
     </row>
     <row r="42" spans="1:14">
       <c r="B42" s="11"/>
       <c r="F42" s="18" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H42" s="18" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="M42" s="14"/>
     </row>
     <row r="43" spans="1:14" customHeight="1" ht="13.5">
       <c r="B43" s="11" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F43" s="47" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H43" s="33"/>
       <c r="I43" s="33"/>
@@ -1572,10 +1575,10 @@
     </row>
     <row r="45" spans="1:14" customHeight="1" ht="13.5">
       <c r="B45" s="11" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F45" s="47" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H45" s="33"/>
       <c r="I45" s="33"/>
@@ -1590,10 +1593,10 @@
     </row>
     <row r="47" spans="1:14" customHeight="1" ht="13.5">
       <c r="B47" s="11" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F47" s="47" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="H47" s="33"/>
       <c r="I47" s="33"/>
@@ -1608,10 +1611,10 @@
     </row>
     <row r="49" spans="1:14" customHeight="1" ht="13.5">
       <c r="B49" s="11" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F49" s="47" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H49" s="33"/>
       <c r="I49" s="33"/>
@@ -1626,10 +1629,10 @@
     </row>
     <row r="51" spans="1:14" customHeight="1" ht="13.5">
       <c r="B51" s="11" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F51" s="47" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H51" s="33"/>
       <c r="I51" s="33"/>
@@ -1678,7 +1681,7 @@
     </row>
     <row r="55" spans="1:14">
       <c r="B55" s="11" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F55" s="18"/>
       <c r="H55" s="18"/>
@@ -1687,19 +1690,19 @@
     <row r="56" spans="1:14" customHeight="1" ht="12">
       <c r="B56" s="11"/>
       <c r="F56" s="18" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H56" s="18" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="M56" s="14"/>
     </row>
     <row r="57" spans="1:14" customHeight="1" ht="13.5">
       <c r="B57" s="11" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F57" s="47" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H57" s="33"/>
       <c r="I57" s="33"/>
@@ -1715,10 +1718,10 @@
     </row>
     <row r="59" spans="1:14" customHeight="1" ht="13.5">
       <c r="B59" s="11" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F59" s="47" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="H59" s="33"/>
       <c r="I59" s="33"/>
@@ -1734,10 +1737,10 @@
     </row>
     <row r="61" spans="1:14" customHeight="1" ht="13.5">
       <c r="B61" s="11" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F61" s="47" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H61" s="33"/>
       <c r="I61" s="33"/>
@@ -1753,10 +1756,10 @@
     </row>
     <row r="63" spans="1:14" customHeight="1" ht="13.5">
       <c r="B63" s="11" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F63" s="47" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H63" s="33"/>
       <c r="I63" s="33"/>
@@ -1772,10 +1775,10 @@
     </row>
     <row r="65" spans="1:14" customHeight="1" ht="13.5">
       <c r="B65" s="11" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F65" s="47" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H65" s="33"/>
       <c r="I65" s="33"/>
@@ -1791,10 +1794,10 @@
     </row>
     <row r="67" spans="1:14" customHeight="1" ht="13.5">
       <c r="B67" s="11" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F67" s="47" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="H67" s="33"/>
       <c r="I67" s="33"/>
@@ -1809,7 +1812,7 @@
     </row>
     <row r="69" spans="1:14">
       <c r="B69" s="11" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F69" s="33"/>
       <c r="H69" s="33"/>
@@ -1851,19 +1854,19 @@
     <row r="73" spans="1:14">
       <c r="A73" s="18"/>
       <c r="B73" s="58" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C73" s="59"/>
       <c r="D73" s="18"/>
       <c r="E73" s="18"/>
       <c r="F73" s="59" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G73" s="59"/>
       <c r="H73" s="59"/>
       <c r="I73" s="59"/>
       <c r="L73" s="59" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="M73" s="60"/>
     </row>
@@ -1894,13 +1897,13 @@
       <c r="D76" s="18"/>
       <c r="E76" s="18"/>
       <c r="F76" s="51" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G76" s="51"/>
       <c r="H76" s="51"/>
       <c r="I76" s="51"/>
       <c r="L76" s="51" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="M76" s="52"/>
     </row>

</xml_diff>